<commit_message>
Updates + meeting notes
</commit_message>
<xml_diff>
--- a/Users/pbrown/New Member Project/BOM.xlsx
+++ b/Users/pbrown/New Member Project/BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Line Item</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>573-B or 543-B</t>
+  </si>
+  <si>
+    <t>Launch lugs</t>
+  </si>
+  <si>
+    <t>1" Rail Button for 1010 rail</t>
+  </si>
+  <si>
+    <t>Apogee</t>
+  </si>
+  <si>
+    <t>https://www.apogeerockets.com/Building_Supplies/Rail_Buttons/1in_1010_Rail_Button_Standard</t>
   </si>
 </sst>
 </file>
@@ -281,7 +293,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -294,6 +306,9 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -600,17 +615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.75" bestFit="1" customWidth="1"/>
@@ -832,63 +847,67 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3.22</v>
+      </c>
+      <c r="D8" s="10">
+        <v>13060</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="8"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>36</v>
@@ -898,19 +917,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>36</v>
@@ -920,45 +939,47 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="8"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -967,7 +988,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
@@ -978,14 +999,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
@@ -996,14 +1019,14 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="8"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
@@ -1014,16 +1037,14 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="8"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
@@ -1034,25 +1055,51 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
       <c r="C19" s="8"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="9">
+        <f>SUM(C2:C7)</f>
+        <v>231.77999999999997</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1062,8 +1109,9 @@
     <hyperlink ref="J5" r:id="rId4"/>
     <hyperlink ref="J6" r:id="rId5"/>
     <hyperlink ref="J7" r:id="rId6" location="floatingcart_a"/>
+    <hyperlink ref="J8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New Member Project updates
</commit_message>
<xml_diff>
--- a/Users/pbrown/New Member Project/BOM.xlsx
+++ b/Users/pbrown/New Member Project/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Line Item</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Home Depot</t>
   </si>
   <si>
-    <t>3/16" balsa</t>
-  </si>
-  <si>
     <t>On hand</t>
   </si>
   <si>
@@ -143,15 +140,6 @@
   </si>
   <si>
     <t>CR-3.0-2.1 2PK</t>
-  </si>
-  <si>
-    <t>3/16" x 1.25" eye bolt</t>
-  </si>
-  <si>
-    <t>3/16" washer</t>
-  </si>
-  <si>
-    <t>3/16" nut</t>
   </si>
   <si>
     <t>Motor</t>
@@ -204,6 +192,36 @@
   </si>
   <si>
     <t>https://www.apogeerockets.com/Building_Supplies/Rail_Buttons/1in_1010_Rail_Button_Standard</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>1/4" Birch Ply</t>
+  </si>
+  <si>
+    <t>Pro54-4G casing</t>
+  </si>
+  <si>
+    <t>Epoxy Filler</t>
+  </si>
+  <si>
+    <t>404 high density sdhesive filler</t>
+  </si>
+  <si>
+    <t>1/4"" x 1.25" eye bolt</t>
+  </si>
+  <si>
+    <t>1/4" washer</t>
+  </si>
+  <si>
+    <t>1/4" nut</t>
+  </si>
+  <si>
+    <t>1/8" balsa</t>
+  </si>
+  <si>
+    <t>K650</t>
   </si>
 </sst>
 </file>
@@ -615,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,13 +647,14 @@
     <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.75" customWidth="1"/>
+    <col min="8" max="8" width="69.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -654,20 +673,21 @@
       <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -684,20 +704,21 @@
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -714,20 +735,21 @@
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -738,26 +760,27 @@
         <v>6.95</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="2"/>
+      <c r="K4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -776,20 +799,21 @@
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -800,26 +824,27 @@
         <v>152.94999999999999</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -831,23 +856,26 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -861,19 +889,20 @@
         <v>13060</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -885,121 +914,125 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="8"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
         <v>8</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2">
-        <v>4</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="8"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
@@ -1008,108 +1041,159 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="H16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="8"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>16</v>
-      </c>
-      <c r="B19" s="2">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="8"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>17</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
       <c r="C20" s="8"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="9">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="9">
         <f>SUM(C2:C7)</f>
         <v>231.77999999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J4" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6" location="floatingcart_a"/>
-    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K4" r:id="rId2"/>
+    <hyperlink ref="K3" r:id="rId3"/>
+    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="K6" r:id="rId5"/>
+    <hyperlink ref="K7" r:id="rId6" location="floatingcart_a"/>
+    <hyperlink ref="K8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>